<commit_message>
Fixing issues after dasboard split + rename
</commit_message>
<xml_diff>
--- a/episomer/inst/extdata/alert-training.xlsx
+++ b/episomer/inst/extdata/alert-training.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Alerts" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,16 +35,16 @@
     <t xml:space="preserve">Top words</t>
   </si>
   <si>
-    <t xml:space="preserve">Tweets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Top Tweets</t>
+    <t xml:space="preserve">Posts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top Posts</t>
   </si>
   <si>
     <t xml:space="preserve">Given Category</t>
   </si>
   <si>
-    <t xml:space="preserve">Epitweetr Category</t>
+    <t xml:space="preserve">Episomer Category</t>
   </si>
   <si>
     <t xml:space="preserve">Ranking</t>
@@ -247,6 +247,44 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF860D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF222222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDE59"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF3D3D3D"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -318,10 +356,10 @@
     <tableColumn id="2" name="Topic"/>
     <tableColumn id="3" name="Region"/>
     <tableColumn id="4" name="Top words"/>
-    <tableColumn id="5" name="Tweets"/>
-    <tableColumn id="6" name="Top Tweets"/>
+    <tableColumn id="5" name="Posts"/>
+    <tableColumn id="6" name="Top Posts"/>
     <tableColumn id="7" name="Given Category"/>
-    <tableColumn id="8" name="Epitweetr Category"/>
+    <tableColumn id="8" name="Episomer Category"/>
   </tableColumns>
 </table>
 </file>
@@ -354,13 +392,13 @@
   </sheetPr>
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="50.71"/>
@@ -895,8 +933,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -914,13 +952,13 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -1079,8 +1117,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>